<commit_message>
Location type column added
</commit_message>
<xml_diff>
--- a/data/Indoor plants.xlsx
+++ b/data/Indoor plants.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stuuobedu-my.sharepoint.com/personal/landscape_uob_edu_bh/Documents/Indoor plants/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\landscapingUOB-api\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2624" documentId="13_ncr:1_{1A78217F-71DB-4EFB-86F2-DBB25A633962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{35355CA5-D098-4BA2-8845-D7779A99922C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E51904-FA6D-459D-B4DE-8583A33F7B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -443,7 +443,7 @@
         <b/>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -608,7 +608,7 @@
         <b/>
         <sz val="12"/>
         <color rgb="FF000000"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -1090,18 +1090,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1109,68 +1109,68 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF242424"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF242424"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1201,7 +1201,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1261,7 +1261,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2450,21 +2449,21 @@
       <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.875" style="9"/>
-    <col min="2" max="2" width="33.875" style="9" customWidth="1"/>
-    <col min="3" max="3" width="42.75" style="9" customWidth="1"/>
+    <col min="1" max="1" width="8.90625" style="9"/>
+    <col min="2" max="2" width="33.90625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="42.7265625" style="9" customWidth="1"/>
     <col min="4" max="4" width="22" style="9" customWidth="1"/>
-    <col min="5" max="5" width="67.5" style="9" customWidth="1"/>
-    <col min="6" max="6" width="32.5" style="12" customWidth="1"/>
+    <col min="5" max="5" width="67.453125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="32.453125" style="12" customWidth="1"/>
     <col min="7" max="7" width="20" style="9" customWidth="1"/>
-    <col min="8" max="8" width="21.375" style="9" customWidth="1"/>
-    <col min="9" max="9" width="70.875" style="9" customWidth="1"/>
-    <col min="10" max="16384" width="8.875" style="9"/>
+    <col min="8" max="8" width="21.36328125" style="9" customWidth="1"/>
+    <col min="9" max="9" width="70.90625" style="9" customWidth="1"/>
+    <col min="10" max="16384" width="8.90625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="7" customFormat="1">
+    <row r="1" spans="1:9" s="7" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2493,7 +2492,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="7" customFormat="1">
+    <row r="2" spans="1:9" s="7" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
@@ -2523,7 +2522,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>17</v>
       </c>
@@ -2553,7 +2552,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>23</v>
       </c>
@@ -2583,7 +2582,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="17.25" customHeight="1">
+    <row r="5" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>29</v>
       </c>
@@ -2613,7 +2612,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="16.5" customHeight="1">
+    <row r="6" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>34</v>
       </c>
@@ -2643,7 +2642,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>40</v>
       </c>
@@ -2673,7 +2672,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
         <v>46</v>
       </c>
@@ -2703,7 +2702,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
         <v>52</v>
       </c>
@@ -2733,7 +2732,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>57</v>
       </c>
@@ -2763,7 +2762,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>62</v>
       </c>
@@ -2793,7 +2792,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
         <v>68</v>
       </c>
@@ -2823,7 +2822,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
         <v>74</v>
       </c>
@@ -2853,7 +2852,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
         <v>79</v>
       </c>
@@ -2883,7 +2882,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
         <v>85</v>
       </c>
@@ -2913,7 +2912,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
         <v>91</v>
       </c>
@@ -2943,7 +2942,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
         <v>96</v>
       </c>
@@ -2973,7 +2972,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
         <v>101</v>
       </c>
@@ -3003,7 +3002,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
         <v>107</v>
       </c>
@@ -3033,7 +3032,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
         <v>113</v>
       </c>
@@ -3063,7 +3062,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
         <v>118</v>
       </c>
@@ -3093,7 +3092,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
         <v>125</v>
       </c>
@@ -3123,7 +3122,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.75">
+    <row r="23" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="s">
         <v>130</v>
       </c>
@@ -3153,7 +3152,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="s">
         <v>135</v>
       </c>
@@ -3183,7 +3182,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="8" t="s">
         <v>140</v>
       </c>
@@ -3213,7 +3212,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="8" t="s">
         <v>145</v>
       </c>
@@ -3243,7 +3242,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="8" t="s">
         <v>150</v>
       </c>
@@ -3273,7 +3272,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="8" t="s">
         <v>155</v>
       </c>
@@ -3303,7 +3302,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A29" s="8" t="s">
         <v>160</v>
       </c>
@@ -3333,7 +3332,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A30" s="8" t="s">
         <v>166</v>
       </c>
@@ -3363,7 +3362,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A31" s="8" t="s">
         <v>171</v>
       </c>
@@ -3393,7 +3392,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" s="8" t="s">
         <v>176</v>
       </c>
@@ -3423,7 +3422,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="15.75">
+    <row r="33" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A33" s="8" t="s">
         <v>181</v>
       </c>
@@ -3453,7 +3452,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A34" s="8" t="s">
         <v>186</v>
       </c>
@@ -3483,7 +3482,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A35" s="8" t="s">
         <v>191</v>
       </c>
@@ -3513,7 +3512,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A36" s="8" t="s">
         <v>196</v>
       </c>
@@ -3543,7 +3542,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A37" s="8" t="s">
         <v>202</v>
       </c>
@@ -3573,7 +3572,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A38" s="8" t="s">
         <v>208</v>
       </c>
@@ -3603,7 +3602,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A39" s="8" t="s">
         <v>213</v>
       </c>
@@ -3633,7 +3632,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="14.25" customHeight="1">
+    <row r="40" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="8" t="s">
         <v>219</v>
       </c>
@@ -3663,7 +3662,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A41" s="8" t="s">
         <v>224</v>
       </c>
@@ -3693,7 +3692,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A42" s="8" t="s">
         <v>229</v>
       </c>
@@ -3723,7 +3722,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A43" s="8" t="s">
         <v>234</v>
       </c>
@@ -3753,7 +3752,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A44" s="8" t="s">
         <v>239</v>
       </c>
@@ -3783,7 +3782,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A45" s="8" t="s">
         <v>244</v>
       </c>
@@ -3813,7 +3812,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A46" s="8" t="s">
         <v>249</v>
       </c>
@@ -3843,7 +3842,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A47" s="8" t="s">
         <v>254</v>
       </c>
@@ -3873,7 +3872,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A48" s="8" t="s">
         <v>259</v>
       </c>
@@ -3903,7 +3902,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A49" s="8" t="s">
         <v>264</v>
       </c>
@@ -3933,7 +3932,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A50" s="8" t="s">
         <v>269</v>
       </c>
@@ -3963,7 +3962,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A51" s="8" t="s">
         <v>274</v>
       </c>
@@ -3993,7 +3992,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A52" s="8" t="s">
         <v>279</v>
       </c>
@@ -4023,7 +4022,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A53" s="8" t="s">
         <v>284</v>
       </c>
@@ -4053,7 +4052,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="15.75" customHeight="1">
+    <row r="54" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="8" t="s">
         <v>289</v>
       </c>
@@ -4083,7 +4082,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A55" s="8"/>
       <c r="B55" s="22"/>
       <c r="C55" s="22"/>
@@ -4091,147 +4090,147 @@
       <c r="E55" s="13"/>
       <c r="H55" s="22"/>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A56" s="8"/>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A57" s="8"/>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A58" s="8"/>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A59" s="8"/>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A60" s="8"/>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A61" s="8"/>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A62" s="8"/>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A63" s="8"/>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A64" s="8"/>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A65" s="8"/>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A66" s="8"/>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A67" s="8"/>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A68" s="8"/>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A69" s="8"/>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A70" s="8"/>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A71" s="8"/>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A72" s="8"/>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A73" s="8"/>
     </row>
-    <row r="74" spans="1:1">
+    <row r="74" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A74" s="8"/>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A75" s="8"/>
     </row>
-    <row r="76" spans="1:1">
+    <row r="76" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A76" s="8"/>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A77" s="8"/>
     </row>
-    <row r="78" spans="1:1">
+    <row r="78" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A78" s="8"/>
     </row>
-    <row r="79" spans="1:1">
+    <row r="79" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A79" s="8"/>
     </row>
-    <row r="80" spans="1:1">
+    <row r="80" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A80" s="8"/>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A81" s="8"/>
     </row>
-    <row r="82" spans="1:1">
+    <row r="82" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A82" s="8"/>
     </row>
-    <row r="83" spans="1:1">
+    <row r="83" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A83" s="8"/>
     </row>
-    <row r="84" spans="1:1">
+    <row r="84" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A84" s="8"/>
     </row>
-    <row r="85" spans="1:1">
+    <row r="85" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A85" s="8"/>
     </row>
-    <row r="86" spans="1:1">
+    <row r="86" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A86" s="8"/>
     </row>
-    <row r="87" spans="1:1">
+    <row r="87" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A87" s="8"/>
     </row>
-    <row r="88" spans="1:1">
+    <row r="88" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A88" s="8"/>
     </row>
-    <row r="89" spans="1:1">
+    <row r="89" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A89" s="8"/>
     </row>
-    <row r="90" spans="1:1">
+    <row r="90" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A90" s="8"/>
     </row>
-    <row r="91" spans="1:1">
+    <row r="91" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A91" s="8"/>
     </row>
-    <row r="92" spans="1:1">
+    <row r="92" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A92" s="8"/>
     </row>
-    <row r="93" spans="1:1">
+    <row r="93" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A93" s="8"/>
     </row>
-    <row r="94" spans="1:1">
+    <row r="94" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A94" s="8"/>
     </row>
-    <row r="95" spans="1:1">
+    <row r="95" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A95" s="8"/>
     </row>
-    <row r="96" spans="1:1">
+    <row r="96" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A96" s="8"/>
     </row>
-    <row r="97" spans="1:1">
+    <row r="97" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A97" s="8"/>
     </row>
-    <row r="98" spans="1:1">
+    <row r="98" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A98" s="8"/>
     </row>
-    <row r="99" spans="1:1">
+    <row r="99" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A99" s="8"/>
     </row>
-    <row r="100" spans="1:1">
+    <row r="100" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A100" s="8"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B51">
+    <cfRule type="duplicateValues" dxfId="89" priority="91"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B54 B1:B26 B48:B50 B31:B46 B52 B56:B1048576">
-    <cfRule type="duplicateValues" dxfId="89" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B51">
-    <cfRule type="duplicateValues" dxfId="88" priority="91"/>
+    <cfRule type="duplicateValues" dxfId="88" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G35 G37:G1048576" xr:uid="{84F914E3-C5A8-4843-B3F4-1A37C7AF587E}">
@@ -4359,27 +4358,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F66040A-D2D7-471A-B740-24F7C5D64244}">
-  <dimension ref="A1:G165"/>
+  <dimension ref="A1:G164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A154" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E155" sqref="E155"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F172" sqref="F172"/>
+      <selection pane="bottomLeft" sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.25" style="2" customWidth="1"/>
-    <col min="2" max="2" width="38.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="19.625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="48.5" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="145.625" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.875" style="2"/>
+    <col min="1" max="1" width="12.26953125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="38.453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.08984375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="19.6328125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="48.453125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.08984375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="145.6328125" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.90625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -4399,7 +4398,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="str">
         <f>_xlfn.XLOOKUP(B2, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-001</v>
@@ -4421,7 +4420,7 @@
       </c>
       <c r="G2" s="27"/>
     </row>
-    <row r="3" spans="1:7" ht="15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="str">
         <f>_xlfn.XLOOKUP(B3, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-002</v>
@@ -4442,7 +4441,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="str">
         <f>_xlfn.XLOOKUP(B4, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-003</v>
@@ -4463,7 +4462,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="str">
         <f>_xlfn.XLOOKUP(B5, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-005</v>
@@ -4484,7 +4483,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="str">
         <f>_xlfn.XLOOKUP(B6, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-008</v>
@@ -4505,7 +4504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="str">
         <f>_xlfn.XLOOKUP(B7, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-009</v>
@@ -4526,7 +4525,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="str">
         <f>_xlfn.XLOOKUP(B8, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-010</v>
@@ -4547,7 +4546,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="str">
         <f>_xlfn.XLOOKUP(B9, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-011</v>
@@ -4568,7 +4567,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="str">
         <f>_xlfn.XLOOKUP(B10, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-013</v>
@@ -4589,7 +4588,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="str">
         <f>_xlfn.XLOOKUP(B11, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-014</v>
@@ -4610,7 +4609,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="str">
         <f>_xlfn.XLOOKUP(B12, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-015</v>
@@ -4631,7 +4630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="str">
         <f>_xlfn.XLOOKUP(B13, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-016</v>
@@ -4652,7 +4651,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="str">
         <f>_xlfn.XLOOKUP(B14, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-019</v>
@@ -4673,7 +4672,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="str">
         <f>_xlfn.XLOOKUP(B15, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-021</v>
@@ -4694,7 +4693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="str">
         <f>_xlfn.XLOOKUP(B16, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-022</v>
@@ -4715,7 +4714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="str">
         <f>_xlfn.XLOOKUP(B17, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-023</v>
@@ -4736,7 +4735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="str">
         <f>_xlfn.XLOOKUP(B18, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-024</v>
@@ -4757,7 +4756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="str">
         <f>_xlfn.XLOOKUP(B19, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-025</v>
@@ -4778,7 +4777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="str">
         <f>_xlfn.XLOOKUP(B20, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-030</v>
@@ -4799,7 +4798,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="str">
         <f>_xlfn.XLOOKUP(B21, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-031</v>
@@ -4820,7 +4819,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="str">
         <f>_xlfn.XLOOKUP(B22, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-032</v>
@@ -4841,7 +4840,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="str">
         <f>_xlfn.XLOOKUP(B23, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-033</v>
@@ -4862,7 +4861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="str">
         <f>_xlfn.XLOOKUP(B24, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-034</v>
@@ -4883,7 +4882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="str">
         <f>_xlfn.XLOOKUP(B25, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-035</v>
@@ -4904,7 +4903,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="str">
         <f>_xlfn.XLOOKUP(B26, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-047</v>
@@ -4925,7 +4924,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="str">
         <f>_xlfn.XLOOKUP(B27, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-031</v>
@@ -4946,7 +4945,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="str">
         <f>_xlfn.XLOOKUP(B28, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-005</v>
@@ -4967,7 +4966,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="str">
         <f>_xlfn.XLOOKUP(B29, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-005</v>
@@ -4988,7 +4987,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="str">
         <f>_xlfn.XLOOKUP(B30, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-009</v>
@@ -5009,7 +5008,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="str">
         <f>_xlfn.XLOOKUP(B31, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-016</v>
@@ -5030,7 +5029,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="str">
         <f>_xlfn.XLOOKUP(B32, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-047</v>
@@ -5051,7 +5050,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="str">
         <f>_xlfn.XLOOKUP(B33, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-010</v>
@@ -5072,7 +5071,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="str">
         <f>_xlfn.XLOOKUP(B34, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-005</v>
@@ -5093,7 +5092,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="str">
         <f>_xlfn.XLOOKUP(B35, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-020</v>
@@ -5114,7 +5113,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="str">
         <f>_xlfn.XLOOKUP(B36, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-010</v>
@@ -5135,7 +5134,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="str">
         <f>_xlfn.XLOOKUP(B37, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-016</v>
@@ -5156,7 +5155,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="str">
         <f>_xlfn.XLOOKUP(B38, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-031</v>
@@ -5177,7 +5176,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="str">
         <f>_xlfn.XLOOKUP(B39, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-036</v>
@@ -5198,7 +5197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="str">
         <f>_xlfn.XLOOKUP(B40, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-004</v>
@@ -5219,7 +5218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="str">
         <f>_xlfn.XLOOKUP(B41, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-005</v>
@@ -5240,7 +5239,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="str">
         <f>_xlfn.XLOOKUP(B42, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-005</v>
@@ -5261,7 +5260,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="str">
         <f>_xlfn.XLOOKUP(B43, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-014</v>
@@ -5282,7 +5281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="str">
         <f>_xlfn.XLOOKUP(B44, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-020</v>
@@ -5303,7 +5302,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="str">
         <f>_xlfn.XLOOKUP(B45, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-009</v>
@@ -5324,7 +5323,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="str">
         <f>_xlfn.XLOOKUP(B46, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-031</v>
@@ -5345,7 +5344,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="15">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="str">
         <f>_xlfn.XLOOKUP(B47, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-005</v>
@@ -5366,7 +5365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="str">
         <f>_xlfn.XLOOKUP(B48, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-019</v>
@@ -5387,7 +5386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="str">
         <f>_xlfn.XLOOKUP(B49, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-003</v>
@@ -5408,7 +5407,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="15">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="str">
         <f>_xlfn.XLOOKUP(B50, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-005</v>
@@ -5429,7 +5428,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="15">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="str">
         <f>_xlfn.XLOOKUP(B51, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-031</v>
@@ -5450,7 +5449,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="str">
         <f>_xlfn.XLOOKUP(B52, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-016</v>
@@ -5471,7 +5470,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="str">
         <f>_xlfn.XLOOKUP(B53, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-013</v>
@@ -5492,7 +5491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="str">
         <f>_xlfn.XLOOKUP(B54, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-047</v>
@@ -5513,7 +5512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="str">
         <f>_xlfn.XLOOKUP(B55, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-005</v>
@@ -5534,7 +5533,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="str">
         <f>_xlfn.XLOOKUP(B56, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-020</v>
@@ -5555,7 +5554,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="str">
         <f>_xlfn.XLOOKUP(B57, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-019</v>
@@ -5576,7 +5575,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="str">
         <f>_xlfn.XLOOKUP(B58, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-005</v>
@@ -5597,7 +5596,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="15">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="str">
         <f>_xlfn.XLOOKUP(B59, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-020</v>
@@ -5618,7 +5617,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="15">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="str">
         <f>_xlfn.XLOOKUP(B60, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-019</v>
@@ -5639,7 +5638,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="15">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="str">
         <f>_xlfn.XLOOKUP(B61, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-014</v>
@@ -5660,7 +5659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="15">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="str">
         <f>_xlfn.XLOOKUP(B62, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-040</v>
@@ -5681,7 +5680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="15">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="str">
         <f>_xlfn.XLOOKUP(B63, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-010</v>
@@ -5702,7 +5701,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="15">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="str">
         <f>_xlfn.XLOOKUP(B64, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-019</v>
@@ -5723,7 +5722,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="15">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="str">
         <f>_xlfn.XLOOKUP(B65, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-031</v>
@@ -5744,7 +5743,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="15">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="str">
         <f>_xlfn.XLOOKUP(B66, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-014</v>
@@ -5765,7 +5764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="15">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="str">
         <f>_xlfn.XLOOKUP(B67, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-005</v>
@@ -5786,7 +5785,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="15">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="str">
         <f>_xlfn.XLOOKUP(B68, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-014</v>
@@ -5807,7 +5806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="15">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="str">
         <f>_xlfn.XLOOKUP(B69, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-019</v>
@@ -5828,7 +5827,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="15">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="str">
         <f>_xlfn.XLOOKUP(B70, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-031</v>
@@ -5849,7 +5848,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="15">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="str">
         <f>_xlfn.XLOOKUP(B71, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-016</v>
@@ -5870,7 +5869,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="15">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="str">
         <f>_xlfn.XLOOKUP(B72, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-036</v>
@@ -5891,7 +5890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="15">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="str">
         <f>_xlfn.XLOOKUP(B73, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-019</v>
@@ -5912,7 +5911,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="15">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="str">
         <f>_xlfn.XLOOKUP(B74, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-031</v>
@@ -5933,7 +5932,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="15">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="str">
         <f>_xlfn.XLOOKUP(B75, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-020</v>
@@ -5954,7 +5953,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="15">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="str">
         <f>_xlfn.XLOOKUP(B76, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-014</v>
@@ -5975,7 +5974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="15">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="str">
         <f>_xlfn.XLOOKUP(B77, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-020</v>
@@ -5996,7 +5995,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="15">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="str">
         <f>_xlfn.XLOOKUP(B78, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-014</v>
@@ -6017,7 +6016,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="15">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="str">
         <f>_xlfn.XLOOKUP(B79, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-016</v>
@@ -6038,7 +6037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="15">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="str">
         <f>_xlfn.XLOOKUP(B80, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-045</v>
@@ -6059,7 +6058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="15">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" s="2" t="str">
         <f>_xlfn.XLOOKUP(B81, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-007</v>
@@ -6080,7 +6079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="15">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82" s="2" t="str">
         <f>_xlfn.XLOOKUP(B82, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-019</v>
@@ -6101,7 +6100,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="15">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" s="2" t="str">
         <f>_xlfn.XLOOKUP(B83, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-010</v>
@@ -6122,7 +6121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="15">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" s="2" t="str">
         <f>_xlfn.XLOOKUP(B84, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-009</v>
@@ -6143,7 +6142,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="15">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" s="2" t="str">
         <f>_xlfn.XLOOKUP(B85, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-007</v>
@@ -6164,7 +6163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="15">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" s="2" t="str">
         <f>_xlfn.XLOOKUP(B86, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-036</v>
@@ -6185,7 +6184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="15">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" s="2" t="str">
         <f>_xlfn.XLOOKUP(B87, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-035</v>
@@ -6206,7 +6205,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="15">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" s="2" t="str">
         <f>_xlfn.XLOOKUP(B88, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-036</v>
@@ -6227,7 +6226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="15">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" s="2" t="str">
         <f>_xlfn.XLOOKUP(B89, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-005</v>
@@ -6248,7 +6247,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="15">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" s="2" t="str">
         <f>_xlfn.XLOOKUP(B90, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-002</v>
@@ -6269,7 +6268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="15">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" s="2" t="str">
         <f>_xlfn.XLOOKUP(B91, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-019</v>
@@ -6290,7 +6289,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="15">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" s="2" t="str">
         <f>_xlfn.XLOOKUP(B92, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-039</v>
@@ -6311,7 +6310,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="15">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" s="2" t="str">
         <f>_xlfn.XLOOKUP(B93, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-005</v>
@@ -6332,7 +6331,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="15">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94" s="2" t="str">
         <f>_xlfn.XLOOKUP(B94, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-046</v>
@@ -6353,7 +6352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="15">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" s="2" t="str">
         <f>_xlfn.XLOOKUP(B95, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-040</v>
@@ -6374,7 +6373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="15">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96" s="2" t="str">
         <f>_xlfn.XLOOKUP(B96, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-036</v>
@@ -6395,7 +6394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="15">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" s="2" t="str">
         <f>_xlfn.XLOOKUP(B97, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-019</v>
@@ -6416,7 +6415,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="15">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" s="2" t="str">
         <f>_xlfn.XLOOKUP(B98, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-039</v>
@@ -6437,7 +6436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="15">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" s="2" t="str">
         <f>_xlfn.XLOOKUP(B99, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-041</v>
@@ -6458,7 +6457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="15">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" s="2" t="str">
         <f>_xlfn.XLOOKUP(B100, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-040</v>
@@ -6479,7 +6478,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="15">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" s="2" t="str">
         <f>_xlfn.XLOOKUP(B101, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-037</v>
@@ -6500,7 +6499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="15">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" s="2" t="str">
         <f>_xlfn.XLOOKUP(B102, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-020</v>
@@ -6521,7 +6520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="15">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103" s="2" t="str">
         <f>_xlfn.XLOOKUP(B103, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-018</v>
@@ -6542,7 +6541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="15">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" s="2" t="str">
         <f>_xlfn.XLOOKUP(B104, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-019</v>
@@ -6563,7 +6562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="15">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" s="2" t="str">
         <f>_xlfn.XLOOKUP(B105, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-052</v>
@@ -6584,7 +6583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="15">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" s="2" t="str">
         <f>_xlfn.XLOOKUP(B106, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-043</v>
@@ -6605,7 +6604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="15">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" s="2" t="str">
         <f>_xlfn.XLOOKUP(B107, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-036</v>
@@ -6626,7 +6625,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="15">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" s="2" t="str">
         <f>_xlfn.XLOOKUP(B108, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-002</v>
@@ -6647,7 +6646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="15">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" s="2" t="str">
         <f>_xlfn.XLOOKUP(B109, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-039</v>
@@ -6668,7 +6667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="15">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110" s="2" t="str">
         <f>_xlfn.XLOOKUP(B110, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-045</v>
@@ -6689,7 +6688,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="15">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111" s="2" t="str">
         <f>_xlfn.XLOOKUP(B111, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-014</v>
@@ -6710,7 +6709,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="15">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112" s="2" t="str">
         <f>_xlfn.XLOOKUP(B112, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-043</v>
@@ -6731,7 +6730,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="15">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113" s="2" t="str">
         <f>_xlfn.XLOOKUP(B113, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-020</v>
@@ -6752,7 +6751,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="15">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114" s="2" t="str">
         <f>_xlfn.XLOOKUP(B114, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-041</v>
@@ -6773,7 +6772,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="15">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A115" s="2" t="str">
         <f>_xlfn.XLOOKUP(B115, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-031</v>
@@ -6794,7 +6793,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="15">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116" s="2" t="str">
         <f>_xlfn.XLOOKUP(B116, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-005</v>
@@ -6815,7 +6814,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="15">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117" s="2" t="str">
         <f>_xlfn.XLOOKUP(B117, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-042</v>
@@ -6836,7 +6835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="15">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118" s="2" t="str">
         <f>_xlfn.XLOOKUP(B118, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-037</v>
@@ -6857,7 +6856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="15">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119" s="2" t="str">
         <f>_xlfn.XLOOKUP(B119, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-038</v>
@@ -6878,7 +6877,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="15">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120" s="2" t="str">
         <f>_xlfn.XLOOKUP(B120, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-019</v>
@@ -6899,7 +6898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="15">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121" s="2" t="str">
         <f>_xlfn.XLOOKUP(B121, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-017</v>
@@ -6920,7 +6919,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="15">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122" s="2" t="str">
         <f>_xlfn.XLOOKUP(B122, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-035</v>
@@ -6941,7 +6940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="15">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A123" s="2" t="str">
         <f>_xlfn.XLOOKUP(B123, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-032</v>
@@ -6962,7 +6961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:6" ht="15">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124" s="2" t="str">
         <f>_xlfn.XLOOKUP(B124, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-036</v>
@@ -6983,7 +6982,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="125" spans="1:6" ht="15">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A125" s="2" t="str">
         <f>_xlfn.XLOOKUP(B125, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-033</v>
@@ -7004,7 +7003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="15">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A126" s="2" t="str">
         <f>_xlfn.XLOOKUP(B126, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-039</v>
@@ -7025,7 +7024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:6" ht="15">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A127" s="2" t="str">
         <f>_xlfn.XLOOKUP(B127, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-012</v>
@@ -7046,7 +7045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="15">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A128" s="2" t="str">
         <f>_xlfn.XLOOKUP(B128, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-009</v>
@@ -7067,7 +7066,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="129" spans="1:6" ht="15">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A129" s="2" t="str">
         <f>_xlfn.XLOOKUP(B129, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-006</v>
@@ -7088,7 +7087,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="15">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A130" s="2" t="str">
         <f>_xlfn.XLOOKUP(B130, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-003</v>
@@ -7109,7 +7108,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="1:6" ht="15">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A131" s="2" t="str">
         <f>_xlfn.XLOOKUP(B131, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-015</v>
@@ -7130,7 +7129,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="132" spans="1:6" ht="15">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A132" s="2" t="str">
         <f>_xlfn.XLOOKUP(B132, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-014</v>
@@ -7151,7 +7150,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="133" spans="1:6" ht="15">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A133" s="2" t="str">
         <f>_xlfn.XLOOKUP(B133, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-039</v>
@@ -7172,7 +7171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="15">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A134" s="2" t="str">
         <f>_xlfn.XLOOKUP(B134, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-044</v>
@@ -7193,7 +7192,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="1:6" ht="15">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A135" s="2" t="str">
         <f>_xlfn.XLOOKUP(B135, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-036</v>
@@ -7214,7 +7213,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="136" spans="1:6" ht="15">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A136" s="2" t="str">
         <f>_xlfn.XLOOKUP(B136, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-048</v>
@@ -7235,7 +7234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:6" ht="15">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A137" s="2" t="str">
         <f>_xlfn.XLOOKUP(B137, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-009</v>
@@ -7256,7 +7255,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="138" spans="1:6" ht="15">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A138" s="2" t="str">
         <f>_xlfn.XLOOKUP(B138, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-012</v>
@@ -7277,7 +7276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:6" ht="15">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A139" s="2" t="str">
         <f>_xlfn.XLOOKUP(B139, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-049</v>
@@ -7298,7 +7297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:6" ht="15">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A140" s="2" t="str">
         <f>_xlfn.XLOOKUP(B140, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-050</v>
@@ -7319,7 +7318,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="141" spans="1:6" ht="15">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A141" s="2" t="str">
         <f>_xlfn.XLOOKUP(B141, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-051</v>
@@ -7340,7 +7339,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:6" ht="15">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A142" s="2" t="str">
         <f>_xlfn.XLOOKUP(B142, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-026</v>
@@ -7361,7 +7360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:6" ht="15">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A143" s="2" t="str">
         <f>_xlfn.XLOOKUP(B143, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-029</v>
@@ -7382,7 +7381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:6" ht="15">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A144" s="2" t="str">
         <f>_xlfn.XLOOKUP(B144, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-027</v>
@@ -7403,7 +7402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:6" ht="15">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A145" s="2" t="str">
         <f>_xlfn.XLOOKUP(B145, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-028</v>
@@ -7424,7 +7423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:6" ht="15">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A146" s="2" t="str">
         <f>_xlfn.XLOOKUP(B146, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-052</v>
@@ -7445,7 +7444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:6" ht="15">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A147" s="2" t="str">
         <f>_xlfn.XLOOKUP(B147, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-005</v>
@@ -7466,7 +7465,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="148" spans="1:6" ht="15">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A148" s="2" t="str">
         <f>_xlfn.XLOOKUP(B148, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-020</v>
@@ -7487,7 +7486,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="149" spans="1:6" ht="15">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A149" s="2" t="str">
         <f>_xlfn.XLOOKUP(B149, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-048</v>
@@ -7508,7 +7507,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="150" spans="1:6" ht="15">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A150" s="2" t="str">
         <f>_xlfn.XLOOKUP(B150, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-013</v>
@@ -7529,7 +7528,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="151" spans="1:6" ht="15">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A151" s="2" t="str">
         <f>_xlfn.XLOOKUP(B151, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-032</v>
@@ -7550,7 +7549,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="152" spans="1:6" ht="15">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A152" s="2" t="str">
         <f>_xlfn.XLOOKUP(B152, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-014</v>
@@ -7571,7 +7570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:6" ht="15">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A153" s="2" t="str">
         <f>_xlfn.XLOOKUP(B153, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-015</v>
@@ -7592,7 +7591,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="15">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A154" s="2" t="str">
         <f>_xlfn.XLOOKUP(B154, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-044</v>
@@ -7613,28 +7612,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:6" s="29" customFormat="1" ht="15">
-      <c r="A155" s="29" t="str">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A155" s="2" t="str">
         <f>_xlfn.XLOOKUP(B155, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-053</v>
       </c>
-      <c r="B155" s="29" t="s">
+      <c r="B155" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="C155" s="29" t="s">
-        <v>298</v>
-      </c>
-      <c r="D155" s="29" t="s">
+      <c r="C155" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D155" s="2" t="s">
         <v>301</v>
       </c>
       <c r="E155" s="26" t="s">
         <v>339</v>
       </c>
-      <c r="F155" s="29">
+      <c r="F155" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:6" ht="15">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A156" s="2" t="str">
         <f>_xlfn.XLOOKUP(B156, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-043</v>
@@ -7655,7 +7654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:6" ht="15">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A157" s="2" t="str">
         <f>_xlfn.XLOOKUP(B157, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-013</v>
@@ -7676,7 +7675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:6" ht="15">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A158" s="2" t="str">
         <f>_xlfn.XLOOKUP(B158, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-019</v>
@@ -7697,7 +7696,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="159" spans="1:6" ht="15">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A159" s="2" t="str">
         <f>_xlfn.XLOOKUP(B159, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-019</v>
@@ -7718,7 +7717,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="160" spans="1:6" ht="15">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A160" s="2" t="str">
         <f>_xlfn.XLOOKUP(B160, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-008</v>
@@ -7739,7 +7738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:6" ht="15">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A161" s="2" t="str">
         <f>_xlfn.XLOOKUP(B161, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-047</v>
@@ -7760,7 +7759,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="162" spans="1:6" ht="15">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A162" s="2" t="str">
         <f>_xlfn.XLOOKUP(B162, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-032</v>
@@ -7781,7 +7780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:6" ht="15">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A163" s="2" t="str">
         <f>_xlfn.XLOOKUP(B163, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-015</v>
@@ -7802,7 +7801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:6" ht="15">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A164" s="2" t="str">
         <f>_xlfn.XLOOKUP(B164, Sheet1!B:B, Sheet1!A:A, "Not Found")</f>
         <v>IP-005</v>
@@ -7823,7 +7822,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:6" ht="15"/>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:C5">
     <sortCondition ref="B3:B5"/>
@@ -7859,8 +7857,8 @@
     <cfRule type="duplicateValues" dxfId="78" priority="49"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43">
-    <cfRule type="duplicateValues" dxfId="77" priority="30"/>
-    <cfRule type="duplicateValues" dxfId="76" priority="48"/>
+    <cfRule type="duplicateValues" dxfId="77" priority="48"/>
+    <cfRule type="duplicateValues" dxfId="76" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44">
     <cfRule type="duplicateValues" dxfId="75" priority="47"/>
@@ -7875,33 +7873,33 @@
     <cfRule type="duplicateValues" dxfId="72" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48">
-    <cfRule type="duplicateValues" dxfId="71" priority="26"/>
-    <cfRule type="duplicateValues" dxfId="70" priority="90"/>
+    <cfRule type="duplicateValues" dxfId="71" priority="90"/>
+    <cfRule type="duplicateValues" dxfId="70" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B49">
-    <cfRule type="duplicateValues" dxfId="69" priority="25"/>
-    <cfRule type="duplicateValues" dxfId="68" priority="89"/>
+    <cfRule type="duplicateValues" dxfId="69" priority="89"/>
+    <cfRule type="duplicateValues" dxfId="68" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B50">
     <cfRule type="duplicateValues" dxfId="67" priority="66"/>
     <cfRule type="duplicateValues" dxfId="66" priority="88"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B51">
-    <cfRule type="duplicateValues" dxfId="65" priority="24"/>
-    <cfRule type="duplicateValues" dxfId="64" priority="87"/>
+    <cfRule type="duplicateValues" dxfId="65" priority="87"/>
+    <cfRule type="duplicateValues" dxfId="64" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B52">
     <cfRule type="duplicateValues" dxfId="63" priority="23"/>
     <cfRule type="duplicateValues" dxfId="62" priority="65"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B53">
-    <cfRule type="duplicateValues" dxfId="61" priority="22"/>
-    <cfRule type="duplicateValues" dxfId="60" priority="64"/>
+    <cfRule type="duplicateValues" dxfId="61" priority="64"/>
+    <cfRule type="duplicateValues" dxfId="60" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B54">
-    <cfRule type="duplicateValues" dxfId="59" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="59" priority="63"/>
     <cfRule type="duplicateValues" dxfId="58" priority="46"/>
-    <cfRule type="duplicateValues" dxfId="57" priority="63"/>
+    <cfRule type="duplicateValues" dxfId="57" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B55">
     <cfRule type="duplicateValues" dxfId="56" priority="62"/>
@@ -7911,24 +7909,24 @@
     <cfRule type="duplicateValues" dxfId="54" priority="61"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B57">
-    <cfRule type="duplicateValues" dxfId="53" priority="20"/>
-    <cfRule type="duplicateValues" dxfId="52" priority="44"/>
+    <cfRule type="duplicateValues" dxfId="53" priority="44"/>
+    <cfRule type="duplicateValues" dxfId="52" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B58">
     <cfRule type="duplicateValues" dxfId="51" priority="43"/>
     <cfRule type="duplicateValues" dxfId="50" priority="60"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B59">
-    <cfRule type="duplicateValues" dxfId="49" priority="42"/>
-    <cfRule type="duplicateValues" dxfId="48" priority="59"/>
+    <cfRule type="duplicateValues" dxfId="49" priority="59"/>
+    <cfRule type="duplicateValues" dxfId="48" priority="42"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B60">
-    <cfRule type="duplicateValues" dxfId="47" priority="41"/>
-    <cfRule type="duplicateValues" dxfId="46" priority="58"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="58"/>
+    <cfRule type="duplicateValues" dxfId="46" priority="41"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B61">
-    <cfRule type="duplicateValues" dxfId="45" priority="57"/>
-    <cfRule type="duplicateValues" dxfId="44" priority="86"/>
+    <cfRule type="duplicateValues" dxfId="45" priority="86"/>
+    <cfRule type="duplicateValues" dxfId="44" priority="57"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B62">
     <cfRule type="duplicateValues" dxfId="43" priority="40"/>
@@ -7938,14 +7936,14 @@
     <cfRule type="duplicateValues" dxfId="41" priority="85"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B64">
-    <cfRule type="duplicateValues" dxfId="40" priority="19"/>
-    <cfRule type="duplicateValues" dxfId="39" priority="38"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="84"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="19"/>
     <cfRule type="duplicateValues" dxfId="38" priority="56"/>
-    <cfRule type="duplicateValues" dxfId="37" priority="84"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="38"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B65">
-    <cfRule type="duplicateValues" dxfId="36" priority="37"/>
-    <cfRule type="duplicateValues" dxfId="35" priority="83"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="83"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="37"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B66">
     <cfRule type="duplicateValues" dxfId="34" priority="82"/>
@@ -7976,73 +7974,73 @@
   <conditionalFormatting sqref="B82">
     <cfRule type="duplicateValues" dxfId="24" priority="71"/>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B88">
+    <cfRule type="duplicateValues" dxfId="23" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B98">
+    <cfRule type="duplicateValues" dxfId="22" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B99">
+    <cfRule type="duplicateValues" dxfId="21" priority="3"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B112">
-    <cfRule type="duplicateValues" dxfId="23" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B113">
-    <cfRule type="duplicateValues" dxfId="22" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B114">
-    <cfRule type="duplicateValues" dxfId="21" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B115">
-    <cfRule type="duplicateValues" dxfId="20" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B119">
-    <cfRule type="duplicateValues" dxfId="19" priority="54"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="54"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B120">
-    <cfRule type="duplicateValues" dxfId="18" priority="53"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="53"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B121">
-    <cfRule type="duplicateValues" dxfId="17" priority="52"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="52"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B122">
-    <cfRule type="duplicateValues" dxfId="16" priority="51"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="51"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B137">
+    <cfRule type="duplicateValues" dxfId="12" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B146">
+    <cfRule type="duplicateValues" dxfId="11" priority="13"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B147">
+    <cfRule type="duplicateValues" dxfId="10" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B151">
-    <cfRule type="duplicateValues" dxfId="15" priority="74"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="74"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B152">
-    <cfRule type="duplicateValues" dxfId="14" priority="73"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="73"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B153">
-    <cfRule type="duplicateValues" dxfId="13" priority="14"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B146">
-    <cfRule type="duplicateValues" dxfId="12" priority="13"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B147">
-    <cfRule type="duplicateValues" dxfId="11" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B156">
-    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B161">
-    <cfRule type="duplicateValues" dxfId="9" priority="8"/>
-    <cfRule type="duplicateValues" dxfId="8" priority="9"/>
-    <cfRule type="duplicateValues" dxfId="7" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B162">
-    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B163">
-    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B164">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B98">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B99">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B88">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B137">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1 D161:D1048576 D155 D2:D95 D97:D146" xr:uid="{8270B7E8-CE95-4076-B244-68DB0D08C67D}"/>

</xml_diff>